<commit_message>
ER e ER ristr, Relazionale
</commit_message>
<xml_diff>
--- a/06_Relazionale_v2.xlsx
+++ b/06_Relazionale_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danyp\Documents\Programmazione\Basi di Dati - Progetto Gestione Zoo\Progetto-Laboratorio-BSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Basi di Dati - Progetto Gestione Zoo\Progetto-Laboratorio-BSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF1EFB0-C593-4E7B-A3A6-2E95805C25A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D249846D-CFFE-4C65-A9CE-44EAE2E0D332}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5730" yWindow="990" windowWidth="11520" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -982,26 +982,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="15" width="17.6640625" customWidth="1"/>
-    <col min="16" max="21" width="16.88671875" customWidth="1"/>
-    <col min="22" max="28" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="15" width="17.7109375" customWidth="1"/>
+    <col min="16" max="21" width="16.85546875" customWidth="1"/>
+    <col min="22" max="28" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1016,7 +1016,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1031,7 +1031,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="38" t="s">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1087,7 +1087,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="24"/>
       <c r="C7" s="8"/>
@@ -1098,19 +1098,19 @@
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="13"/>
       <c r="K7" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="14"/>
       <c r="C8" s="9"/>
@@ -1125,7 +1125,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -1140,7 +1140,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1155,7 +1155,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1170,7 +1170,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1184,7 +1184,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="38" t="s">
         <v>8</v>
@@ -1203,7 +1203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="12" t="s">
         <v>4</v>
@@ -1233,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="13"/>
       <c r="C15" s="11"/>
@@ -1243,12 +1243,8 @@
       <c r="E15" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>33</v>
-      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="35" t="s">
         <v>33</v>
       </c>
@@ -1257,7 +1253,7 @@
       </c>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="14"/>
       <c r="C16" s="9"/>
@@ -1269,7 +1265,7 @@
       <c r="I16" s="6"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="15"/>
       <c r="C17" s="10"/>
@@ -1285,7 +1281,7 @@
       </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1298,7 +1294,7 @@
       <c r="J18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1313,7 +1309,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1328,7 +1324,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="38" t="s">
         <v>13</v>
@@ -1345,7 +1341,7 @@
       <c r="J21" s="42"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="12" t="s">
         <v>14</v>
@@ -1374,7 +1370,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="13"/>
       <c r="C23" s="35" t="s">
@@ -1395,7 +1391,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="14"/>
       <c r="C24" s="9"/>
@@ -1408,7 +1404,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="15"/>
       <c r="C25" s="10"/>
@@ -1423,7 +1419,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1440,7 +1436,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1455,7 +1451,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1470,7 +1466,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="38" t="s">
         <v>19</v>
@@ -1490,7 +1486,7 @@
       <c r="M29" s="39"/>
       <c r="N29" s="40"/>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="12" t="s">
         <v>14</v>
@@ -1530,7 +1526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="13"/>
       <c r="C31" s="35" t="s">
@@ -1551,10 +1547,14 @@
       <c r="L31" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M31" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="14"/>
       <c r="C32" s="9"/>
@@ -1569,7 +1569,7 @@
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
     </row>
-    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="15"/>
       <c r="C33" s="10"/>
@@ -1584,7 +1584,7 @@
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1594,7 +1594,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1604,7 +1604,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1615,7 +1615,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1630,7 +1630,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1645,7 +1645,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1660,7 +1660,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>